<commit_message>
Fixed bug where pdf files were not getting attached
</commit_message>
<xml_diff>
--- a/Certificate_generator/results.xlsx
+++ b/Certificate_generator/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>SNo</t>
   </si>
@@ -50,25 +50,7 @@
     <t>ABHISHEK SHARMA</t>
   </si>
   <si>
-    <t>AWADHESH KUMAR MAURYA</t>
-  </si>
-  <si>
-    <t>BADAL KUMAR</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>anubhavpatrick@gmail.com</t>
-  </si>
-  <si>
-    <t>vineet.sharma@kiet.edu</t>
-  </si>
-  <si>
-    <t>anubhav.patrick@kiet.edu</t>
   </si>
 </sst>
 </file>
@@ -350,10 +332,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -396,49 +378,12 @@
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3:E4" r:id="rId2" display="anubhavpatrick@gmail.com"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated text field content in main_GUI.py
</commit_message>
<xml_diff>
--- a/Certificate_generator/results.xlsx
+++ b/Certificate_generator/results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>SNo</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>anubhavpatrick@gmail.com</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Priyanka Bhardwaj</t>
+  </si>
+  <si>
+    <t>anubhav.patrick@kiet.edu</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Tishka Gupra</t>
   </si>
 </sst>
 </file>
@@ -104,7 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -116,6 +131,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -332,10 +348,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -381,9 +397,45 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>